<commit_message>
added option for formatted report of statistical values requested by dep. of archaeology of AVCR and added option of signal drift correction
</commit_message>
<xml_diff>
--- a/test_data/sample_data_Element_PARAM.xlsx
+++ b/test_data/sample_data_Element_PARAM.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="35" documentId="8_{1AD42B4F-3169-FC43-A83A-415A0E29EC0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{81069055-BA3B-8F4F-ABF9-906FB1068183}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48BA39CD-AF9F-8B41-9A85-A1A970EF79F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7700" yWindow="460" windowWidth="14400" windowHeight="16240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7700" yWindow="500" windowWidth="14400" windowHeight="16240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="names" sheetId="1" r:id="rId1"/>
@@ -83,52 +83,52 @@
     <t>NIST612</t>
   </si>
   <si>
-    <t>Sx1d_phl_01</t>
-  </si>
-  <si>
-    <t>Sx1d_phl_02</t>
-  </si>
-  <si>
-    <t>Sx1d_phl_03</t>
-  </si>
-  <si>
-    <t>Sx1d_phl_04</t>
-  </si>
-  <si>
-    <t>Sx1d_phl_05</t>
-  </si>
-  <si>
-    <t>Sx1d_phl_06</t>
-  </si>
-  <si>
-    <t>Sx1d_phl_07</t>
-  </si>
-  <si>
-    <t>Sx1d_phl_08</t>
-  </si>
-  <si>
-    <t>ZO4_phl_01</t>
-  </si>
-  <si>
-    <t>ZO4_phl_02</t>
-  </si>
-  <si>
-    <t>ZO4_phl_03</t>
-  </si>
-  <si>
-    <t>ZO4_phl_04</t>
-  </si>
-  <si>
-    <t>ZO4_phl_05</t>
-  </si>
-  <si>
-    <t>ZO4_phl_06</t>
-  </si>
-  <si>
-    <t>ZO4_phl_07</t>
-  </si>
-  <si>
-    <t>ZO4_phl_08</t>
+    <t>Sample_1</t>
+  </si>
+  <si>
+    <t>Sample_2</t>
+  </si>
+  <si>
+    <t>Sample_3</t>
+  </si>
+  <si>
+    <t>Sample_4</t>
+  </si>
+  <si>
+    <t>Sample_5</t>
+  </si>
+  <si>
+    <t>Sample_6</t>
+  </si>
+  <si>
+    <t>Sample_7</t>
+  </si>
+  <si>
+    <t>Sample_8</t>
+  </si>
+  <si>
+    <t>Sample_9</t>
+  </si>
+  <si>
+    <t>Sample_10</t>
+  </si>
+  <si>
+    <t>Sample_11</t>
+  </si>
+  <si>
+    <t>Sample_12</t>
+  </si>
+  <si>
+    <t>Sample_13</t>
+  </si>
+  <si>
+    <t>Sample_14</t>
+  </si>
+  <si>
+    <t>Sample_15</t>
+  </si>
+  <si>
+    <t>Sample_16</t>
   </si>
 </sst>
 </file>
@@ -456,7 +456,7 @@
   <dimension ref="A1:A22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A22"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -582,7 +582,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="A12" sqref="A12:A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>